<commit_message>
Data vis ps2 update
</commit_message>
<xml_diff>
--- a/DATA-VIS/ps2/ps2.xlsx
+++ b/DATA-VIS/ps2/ps2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\DATA-VIS\ps2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A51C7F3F-DA3D-435B-AF2E-AD1C886F780A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CA98F8-DEBF-453B-A1A9-5063B110D3EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{6165F601-D29F-4599-816B-0B7E657B6915}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Men</t>
   </si>
@@ -161,11 +161,92 @@
   <si>
     <t>Dime Bar</t>
   </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>(Urban - City Limits)</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Mumbai (Bombay)</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Dilli (Delhi)</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Korea (South)</t>
+  </si>
+  <si>
+    <t>Sao Paulo</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +351,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -463,6 +550,33 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1087,6 +1201,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F4E1-4AED-B7C7-0A733B223F34}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1129,6 +1248,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F4E1-4AED-B7C7-0A733B223F34}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1171,6 +1295,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F4E1-4AED-B7C7-0A733B223F34}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1213,6 +1342,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F4E1-4AED-B7C7-0A733B223F34}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1255,6 +1389,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F4E1-4AED-B7C7-0A733B223F34}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1297,6 +1436,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F4E1-4AED-B7C7-0A733B223F34}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1577,6 +1721,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1601,6 +1750,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1625,6 +1779,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1649,6 +1808,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1673,6 +1837,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1697,6 +1866,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1723,6 +1897,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1749,6 +1928,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1775,6 +1959,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-E101-40E8-BE42-377D604AF1B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2137,6 +2326,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2161,6 +2355,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2185,6 +2384,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2209,6 +2413,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2233,6 +2442,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2257,6 +2471,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2283,6 +2502,11 @@
               </a:scene3d>
               <a:sp3d prstMaterial="matte"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-AAF6-421F-919E-AC3A6C483E3D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3443,7 +3667,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$108</c15:sqref>
@@ -3471,7 +3695,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$109:$A$118</c15:sqref>
@@ -3515,7 +3739,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$109:$E$118</c15:sqref>
@@ -3558,7 +3782,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-8804-4F6C-853E-670D09FA447A}"/>
                   </c:ext>
@@ -3748,6 +3972,858 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$128:$D$129</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Population</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(Urban - City Limits)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d>
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d>
+                <a:contourClr>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-14DC-499B-A32C-3ACC66447CB8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$130:$C$139</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>China</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>India</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Pakistan</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Argentina</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>India</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Philippines</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Russia</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Korea (South)</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Brazil</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Turkey</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Shanghai</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mumbai (Bombay)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Karachi</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Buenos Aires</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dilli (Delhi)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Manila</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Moscow</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Seoul</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sao Paulo</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Istanbul</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$130:$D$139</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>14608512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12691836</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11624219</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11574205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10927986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10444527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10381222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10349312</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10210295</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9792428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="cone"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-14DC-499B-A32C-3ACC66447CB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1614559823"/>
+        <c:axId val="1606863231"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1614559823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1606863231"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1606863231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1614559823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$148</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$149:$A$158</c:f>
+              <c:numCache>
+                <c:formatCode>_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>23800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$149:$B$158</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-505E-42EE-80DB-3E863B948783}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1480143151"/>
+        <c:axId val="1630714591"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1480143151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1630714591"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1630714591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1480143151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -4029,6 +5105,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -7078,6 +8234,1016 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7315,6 +9481,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>119061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A0B414-1A08-4975-A97E-B326266EA169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{509947F8-1F46-4CFE-8FF8-E592E0ACDCFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7615,16 +9853,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D9AE9F-F74F-4295-9F47-46DD853C5FB1}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="Q129" sqref="Q129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8296,7 +10535,263 @@
         <v>4</v>
       </c>
     </row>
+    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B128" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C128" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D128" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A129" s="29"/>
+      <c r="B129" s="29"/>
+      <c r="C129" s="29"/>
+      <c r="D129" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="26">
+        <v>1</v>
+      </c>
+      <c r="B130" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C130" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D130" s="28">
+        <v>14608512</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="26">
+        <v>2</v>
+      </c>
+      <c r="B131" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C131" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D131" s="28">
+        <v>12691836</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="26">
+        <v>3</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C132" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D132" s="28">
+        <v>11624219</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="26">
+        <v>4</v>
+      </c>
+      <c r="B133" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C133" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D133" s="28">
+        <v>11574205</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="26">
+        <v>5</v>
+      </c>
+      <c r="B134" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C134" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D134" s="28">
+        <v>10927986</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="26">
+        <v>6</v>
+      </c>
+      <c r="B135" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C135" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D135" s="28">
+        <v>10444527</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="26">
+        <v>7</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C136" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D136" s="28">
+        <v>10381222</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="26">
+        <v>8</v>
+      </c>
+      <c r="B137" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C137" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D137" s="28">
+        <v>10349312</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="26">
+        <v>9</v>
+      </c>
+      <c r="B138" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C138" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D138" s="28">
+        <v>10210295</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="26">
+        <v>10</v>
+      </c>
+      <c r="B139" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C139" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D139" s="28">
+        <v>9792428</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="148" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B148" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="33">
+        <v>23800</v>
+      </c>
+      <c r="B149" s="32">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="33">
+        <v>26400</v>
+      </c>
+      <c r="B150" s="32">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="33">
+        <v>23700</v>
+      </c>
+      <c r="B151" s="32">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="33">
+        <v>31900</v>
+      </c>
+      <c r="B152" s="32">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="33">
+        <v>28500</v>
+      </c>
+      <c r="B153" s="32">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="33">
+        <v>32700</v>
+      </c>
+      <c r="B154" s="32">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="33">
+        <v>35700</v>
+      </c>
+      <c r="B155" s="32">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="33">
+        <v>29500</v>
+      </c>
+      <c r="B156" s="32">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="33">
+        <v>37500</v>
+      </c>
+      <c r="B157" s="32">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="33">
+        <v>39700</v>
+      </c>
+      <c r="B158" s="32">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>